<commit_message>
fix a bug in 2a
</commit_message>
<xml_diff>
--- a/logs/2a/2aresult.xlsx
+++ b/logs/2a/2aresult.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -442,502 +442,502 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>299381.0788468003</v>
+        <v>288504.5508113568</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>47042.55646145556</v>
+        <v>37609.82862424095</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>85491.56429633123</v>
+        <v>75565.8528822182</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>83279.37307557097</v>
+        <v>78949.95940588829</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>72903.4983226326</v>
+        <v>61159.02891982916</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>244024.6053370697</v>
+        <v>209731.5255150525</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>79795.64238928095</v>
+        <v>69626.30223623497</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>55344.23924790431</v>
+        <v>46469.70857545878</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>39552.28392091858</v>
+        <v>35696.14385609442</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>68130.91302967831</v>
+        <v>63123.84478749041</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>57038.47153189564</v>
+        <v>53464.91023357871</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>86694.83733595758</v>
+        <v>81342.73572248663</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>88839.07613139835</v>
+        <v>81739.52457452597</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>22489.30428574723</v>
+        <v>19276.85656763474</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>116828.0531266359</v>
+        <v>117630.9536402359</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>105910.4583645574</v>
+        <v>99251.3719825726</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>24504.8516037042</v>
+        <v>15979.75015829244</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>88386.56967018994</v>
+        <v>82927.09302641748</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>51815.50146991827</v>
+        <v>45393.46432031956</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>60335.58069063929</v>
+        <v>64737.73085822884</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>52183.58088947146</v>
+        <v>49632.69356745129</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>45527.63354598637</v>
+        <v>41955.87687536592</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>97074.02649975719</v>
+        <v>86807.04049347091</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>94330.35627892641</v>
+        <v>88327.06810272801</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>13333.95503838355</v>
+        <v>13387.2039112985</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>56699.40502508037</v>
+        <v>52434.92956434948</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>63444.00873655437</v>
+        <v>56425.53542155959</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>85254.34655389268</v>
+        <v>75828.26811740537</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>95806.15337638963</v>
+        <v>78731.49033877561</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>205556.9949644761</v>
+        <v>188366.5224977621</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>73408.79634109377</v>
+        <v>68457.13245405869</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>58277.6772588673</v>
+        <v>64582.49572546703</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>90939.0375700672</v>
+        <v>103908.6745720124</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>118664.5436608392</v>
+        <v>113678.5499176987</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>103989.3605836887</v>
+        <v>94354.3146973332</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>86444.19378274679</v>
+        <v>78231.57813929534</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>94627.28368718742</v>
+        <v>85374.78615633408</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>25187.95753441148</v>
+        <v>22826.92162173722</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>242482.5220682853</v>
+        <v>231684.2522995113</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>96974.06395108305</v>
+        <v>92134.81420432765</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>52675.96238727959</v>
+        <v>49637.13083274924</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>68365.98948614199</v>
+        <v>62466.95265461144</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>52086.79544002518</v>
+        <v>37925.66687774626</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>143824.9967315162</v>
+        <v>127668.1739258605</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>15190.93527914961</v>
+        <v>10681.45704567587</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>57820.32326044638</v>
+        <v>52800.57197574813</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47005.56087947456</v>
+        <v>43846.64443427842</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>61175.27597268061</v>
+        <v>54480.28487128675</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>92056.13531889743</v>
+        <v>105453.8803313497</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>41815.37529909351</v>
+        <v>41732.84436106237</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>72871.10998388618</v>
+        <v>59185.56625616069</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>111971.9517691247</v>
+        <v>105935.0833999371</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>38941.14780620486</v>
+        <v>32639.47633890131</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>38688.58480331256</v>
+        <v>35578.43318048371</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>35380.82743141627</v>
+        <v>28872.66159863357</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>198817.1601786474</v>
+        <v>193509.3354416623</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>45609.7908254817</v>
+        <v>44183.33248351423</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>27027.89199293342</v>
+        <v>20126.40780746128</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>64462.4494996268</v>
+        <v>67991.28610770732</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>114100.4476996032</v>
+        <v>108611.6782937965</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>222138.4320561765</v>
+        <v>215771.5200893505</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>32489.9789100428</v>
+        <v>27211.84075890353</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>213155.6047662821</v>
+        <v>221896.2272498873</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>120590.1175164703</v>
+        <v>116860.7111063749</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>95631.44456292644</v>
+        <v>87068.56717412683</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>97924.62854120594</v>
+        <v>77127.90197223205</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>46937.92356263642</v>
+        <v>51208.20564629497</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>77242.69615313414</v>
+        <v>71891.96432015175</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>104344.5599141879</v>
+        <v>96523.56822806783</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>33202.80506418738</v>
+        <v>28014.64430274286</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>135268.0612946244</v>
+        <v>126663.9479380092</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>33978.74108955764</v>
+        <v>29510.65657633863</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>50671.29074250903</v>
+        <v>51809.78794763309</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>225670.373006893</v>
+        <v>216422.2744131096</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>36600.36150811233</v>
+        <v>29344.22800173918</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>89122.54622875147</v>
+        <v>86325.89188858398</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>52524.79570303026</v>
+        <v>45211.55894453867</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>62031.24383944833</v>
+        <v>70353.6320838845</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>99831.14627278502</v>
+        <v>96143.76320364367</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>49932.09749451531</v>
+        <v>43331.71188431633</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>136903.8207184866</v>
+        <v>145844.8463954173</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>51010.88806798909</v>
+        <v>45967.54278047707</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>50559.76694080715</v>
+        <v>30561.36720004267</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>16429.20966827181</v>
+        <v>20249.21186314673</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>196674.0755374427</v>
+        <v>188687.3793641133</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>88337.65870139055</v>
+        <v>92686.66370008531</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>80159.72337785698</v>
+        <v>86460.60662827775</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>39064.99181741562</v>
+        <v>30336.23770554819</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>47563.3387316028</v>
+        <v>42396.88328025799</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>149468.8757959982</v>
+        <v>142429.2510757815</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>62937.06851211436</v>
+        <v>62840.98370790164</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>31504.89151735899</v>
+        <v>36088.37372944201</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>79114.93394854851</v>
+        <v>78887.39844741176</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>61892.32708851218</v>
+        <v>61317.30057170129</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>374130.329771365</v>
+        <v>367767.7875245648</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>130003.6452603914</v>
+        <v>126952.1394098008</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>63109.58822048221</v>
+        <v>57549.78057554606</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>69797.93235532644</v>
+        <v>63200.69823052623</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>16637.87997544148</v>
+        <v>4925.772066883168</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>63084.33771946804</v>
+        <v>61362.41111483047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>